<commit_message>
Correção de passo na métrica
Cálculo de ECF corrigido
</commit_message>
<xml_diff>
--- a/Diagramas UML/Pontos Caso de Uso.xlsx
+++ b/Diagramas UML/Pontos Caso de Uso.xlsx
@@ -1,12 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="930" yWindow="0" windowWidth="13680" windowHeight="4545"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Página1" sheetId="1" r:id="rId3"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -175,21 +183,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -198,41 +209,307 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.57"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -276,30 +553,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L2" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <f t="shared" ref="N2:N14" si="1">L2*M2</f>
+        <f t="shared" ref="N2:N14" si="0">L2*M2</f>
         <v>0</v>
       </c>
       <c r="P2" s="1" t="s">
@@ -309,37 +586,37 @@
         <v>1.5</v>
       </c>
       <c r="R2" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="S2">
-        <f t="shared" ref="S2:S9" si="2">Q2*R2</f>
+        <f t="shared" ref="S2:S9" si="1">Q2*R2</f>
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M3" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="N3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="P3" s="1" t="s">
@@ -349,19 +626,19 @@
         <v>0.5</v>
       </c>
       <c r="R3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="S3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>17</v>
@@ -374,49 +651,49 @@
         <v>18</v>
       </c>
       <c r="L4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="N4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="Q4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="S4">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="N5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="P5" s="1" t="s">
@@ -426,53 +703,53 @@
         <v>0.5</v>
       </c>
       <c r="R5" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="N6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="Q6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="R6" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="S6">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>27</v>
@@ -481,33 +758,33 @@
         <v>0.5</v>
       </c>
       <c r="M7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="N7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="Q7" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="R7" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="S7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>30</v>
@@ -516,79 +793,79 @@
         <v>0.5</v>
       </c>
       <c r="M8" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="N8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>31</v>
       </c>
       <c r="Q8" s="1">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="R8" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="S8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="L9" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M9" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="N9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="Q9" s="1">
-        <v>-1.0</v>
+        <v>-1</v>
       </c>
       <c r="R9" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="S9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B10" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>36</v>
       </c>
       <c r="L10" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="N10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="P10" s="1" t="s">
@@ -599,98 +876,98 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>39</v>
       </c>
       <c r="L11" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="N11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="Q11">
-        <f>1.4+(0.03*Q10)</f>
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="12">
+        <f>1.4-(0.03*Q10)</f>
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>42</v>
       </c>
       <c r="L12" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="N12">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>44</v>
       </c>
       <c r="L13" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C14" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="L14" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -706,7 +983,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
@@ -719,28 +996,28 @@
       </c>
       <c r="L16">
         <f>0.6+(0.01*L15)</f>
-        <v>0.975</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B17">
         <f>B16*L16*Q11</f>
-        <v>161.304</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>95.315999999999988</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B18">
         <f>B17*20</f>
-        <v>3226.08</v>
+        <v>1906.3199999999997</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fatores Horas/Homem, T4 e E8 alterados
Horas/Homem alterado para 8 baseado em estimativas de tempo final. Fator
de influência de T4 alterado para 1 visto que pouco ou nenhum
processamento complexo será feito. Fator de influência de E8 alterado
para 2 pois a linguagem não é complexa ou desconhecida para os
programadores, ela apenas está inserida em um contexto novo.
</commit_message>
<xml_diff>
--- a/Diagramas UML/Pontos Caso de Uso.xlsx
+++ b/Diagramas UML/Pontos Caso de Uso.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igor6\Documents\GitHub\EngSoft-2017.1-UFJF\Diagramas UML\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -183,8 +183,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -194,13 +194,25 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -212,14 +224,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutra" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -500,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -674,7 +689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -683,18 +698,18 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="1">
-        <v>1</v>
-      </c>
-      <c r="M5" s="1">
-        <v>2</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>22</v>
@@ -813,7 +828,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -834,18 +849,18 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9" s="2">
         <v>-1</v>
       </c>
-      <c r="R9" s="1">
-        <v>5</v>
-      </c>
-      <c r="S9">
+      <c r="R9" s="2">
+        <v>2</v>
+      </c>
+      <c r="S9" s="2">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -873,7 +888,7 @@
       </c>
       <c r="Q10">
         <f>SUM(S2:S9)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -901,7 +916,7 @@
       </c>
       <c r="Q11">
         <f>1.4-(0.03*Q10)</f>
-        <v>1.04</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -980,7 +995,7 @@
       </c>
       <c r="L15">
         <f>SUM(N2:N14)</f>
-        <v>33.5</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
@@ -996,7 +1011,7 @@
       </c>
       <c r="L16">
         <f>0.6+(0.01*L15)</f>
-        <v>0.93500000000000005</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
@@ -1005,7 +1020,7 @@
       </c>
       <c r="B17">
         <f>B16*L16*Q11</f>
-        <v>91.405600000000007</v>
+        <v>82.602499999999992</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
@@ -1013,8 +1028,8 @@
         <v>52</v>
       </c>
       <c r="B18">
-        <f>B17*20</f>
-        <v>1828.1120000000001</v>
+        <f>B17*8</f>
+        <v>660.81999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>